<commit_message>
finalising first edit of all KORA documents
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P2_Preliminary.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P2_Preliminary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601C98BC-1376-47F9-8909-02E960DE5C26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9BE54B-45FB-4A9C-B67F-A2068A9DBEEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10125" xr2:uid="{F66E816F-B844-4025-9D57-703EE86FBE35}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="213">
   <si>
     <t>index</t>
   </si>
@@ -605,6 +605,66 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>AV341</t>
+  </si>
+  <si>
+    <t>oranges, mandarins</t>
+  </si>
+  <si>
+    <t>AV343</t>
+  </si>
+  <si>
+    <t>grapefruits</t>
+  </si>
+  <si>
+    <t>AV344</t>
+  </si>
+  <si>
+    <t>other citrus fruits</t>
+  </si>
+  <si>
+    <t>AV345</t>
+  </si>
+  <si>
+    <t>bananas</t>
+  </si>
+  <si>
+    <t>AV346</t>
+  </si>
+  <si>
+    <t>other tropical fruits</t>
+  </si>
+  <si>
+    <t>AV351</t>
+  </si>
+  <si>
+    <t>nuts</t>
+  </si>
+  <si>
+    <t>AV357</t>
+  </si>
+  <si>
+    <t>dried fruit</t>
+  </si>
+  <si>
+    <t>AV360</t>
+  </si>
+  <si>
+    <t>canned fruit</t>
+  </si>
+  <si>
+    <t>AV370</t>
+  </si>
+  <si>
+    <t>frozen fruit</t>
+  </si>
+  <si>
+    <t>AV390</t>
+  </si>
+  <si>
+    <t>other processed fruit</t>
   </si>
 </sst>
 </file>
@@ -1107,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2CBB1F-BD60-4F64-AB96-FAE7D77C8064}">
   <dimension ref="A1:I304"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2327,44 +2387,144 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="5"/>
-      <c r="D87" s="4"/>
+      <c r="A87">
+        <v>99</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="5"/>
-      <c r="D88" s="5"/>
+      <c r="A88">
+        <v>100</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D88" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="5"/>
-      <c r="D89" s="5"/>
+      <c r="A89">
+        <v>101</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D89" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="5"/>
-      <c r="D90" s="5"/>
+      <c r="A90">
+        <v>102</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D90" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="5"/>
-      <c r="D91" s="4"/>
+      <c r="A91">
+        <v>103</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D91" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="5"/>
-      <c r="D92" s="4"/>
+      <c r="A92">
+        <v>104</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="D92" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="6"/>
-      <c r="D93" s="4"/>
+      <c r="A93">
+        <v>105</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D93" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="5"/>
-      <c r="D94" s="4"/>
+      <c r="A94">
+        <v>106</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D94" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="6"/>
-      <c r="D95" s="5"/>
+      <c r="A95">
+        <v>107</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D95" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="5"/>
-      <c r="D96" s="5"/>
+      <c r="A96">
+        <v>108</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D96" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="6"/>
@@ -4490,6 +4650,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4730,28 +4911,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C5FC19-F4BC-4ACD-86FC-72730E460845}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDB1557E-B519-46C1-8C0E-CA7CA5BBAB79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B441777-EF9E-47A6-A0E0-388F26FE2EA2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4768,23 +4947,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDB1557E-B519-46C1-8C0E-CA7CA5BBAB79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C5FC19-F4BC-4ACD-86FC-72730E460845}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>